<commit_message>
resolución problema con 5 acciones y su frontera eficiente
</commit_message>
<xml_diff>
--- a/retornos.xlsx
+++ b/retornos.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/julio_orozco_uc_cl/Documents/Documents/Portafolios/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_A1E4000D84399E8F98AE09D1FD7AE380E8079D11" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAA3301D-2E91-446A-8520-55F359C95912}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -43,11 +37,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,21 +107,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -165,7 +151,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -199,7 +185,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -234,10 +219,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,17 +394,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -440,1169 +421,1164 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>43861</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>43890</v>
+      </c>
+      <c r="B2">
+        <v>-0.02562298419081355</v>
+      </c>
+      <c r="C2">
+        <v>-0.06663315964807381</v>
+      </c>
+      <c r="D2">
+        <v>-0.1337578366591234</v>
+      </c>
+      <c r="E2">
+        <v>-0.0983035155869324</v>
+      </c>
+      <c r="F2">
+        <v>-0.1107843196269246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>43890</v>
+        <v>43921</v>
       </c>
       <c r="B3">
-        <v>-2.5622817259252861E-2</v>
+        <v>-0.176406106454151</v>
       </c>
       <c r="C3">
-        <v>-6.6633310183274896E-2</v>
+        <v>-0.1000323091794457</v>
       </c>
       <c r="D3">
-        <v>-0.1337580879786063</v>
+        <v>-0.3066176584249773</v>
       </c>
       <c r="E3">
-        <v>-9.8303577266060316E-2</v>
+        <v>-0.1627006246805988</v>
       </c>
       <c r="F3">
-        <v>-0.1107842588019092</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.2282092586875919</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>43921</v>
+        <v>43951</v>
       </c>
       <c r="B4">
-        <v>-0.176406106454151</v>
+        <v>0.02222035539802114</v>
       </c>
       <c r="C4">
-        <v>-0.1000321959439784</v>
+        <v>0.1111113009310669</v>
       </c>
       <c r="D4">
-        <v>-0.30661757325592409</v>
+        <v>0.2089076570210033</v>
       </c>
       <c r="E4">
-        <v>-0.1627004305995903</v>
+        <v>0.1446878528726436</v>
       </c>
       <c r="F4">
-        <v>-0.2282092586875919</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.06487639113176114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>43951</v>
+        <v>43982</v>
       </c>
       <c r="B5">
-        <v>2.2220248654579059E-2</v>
+        <v>0.06885953137199552</v>
       </c>
       <c r="C5">
-        <v>0.11111120961178921</v>
+        <v>-0.1603571459688338</v>
       </c>
       <c r="D5">
-        <v>0.2089077609094554</v>
+        <v>-0.1818380132654362</v>
       </c>
       <c r="E5">
-        <v>0.1446876658414353</v>
+        <v>-0.06242559328925246</v>
       </c>
       <c r="F5">
-        <v>6.4876391131761135E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.03218807996013451</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>43982</v>
+        <v>44012</v>
       </c>
       <c r="B6">
-        <v>6.8859851831926333E-2</v>
+        <v>0.07668732184554083</v>
       </c>
       <c r="C6">
-        <v>-0.16035711718588561</v>
+        <v>0.1833262934444275</v>
       </c>
       <c r="D6">
-        <v>-0.17602760469190021</v>
+        <v>0.39410185858338</v>
       </c>
       <c r="E6">
-        <v>-6.2425593289252457E-2</v>
+        <v>0.03994926994669856</v>
       </c>
       <c r="F6">
-        <v>-3.2188079960134508E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.09108900951825194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>44012</v>
+        <v>44043</v>
       </c>
       <c r="B7">
-        <v>7.6687111469850189E-2</v>
+        <v>0.1718450665745017</v>
       </c>
       <c r="C7">
-        <v>0.18332624690721119</v>
+        <v>-0.04335019089756376</v>
       </c>
       <c r="D7">
-        <v>0.39410187961048287</v>
+        <v>0.03846151611994419</v>
       </c>
       <c r="E7">
-        <v>3.9949193825737472E-2</v>
+        <v>0.04329261468420076</v>
       </c>
       <c r="F7">
-        <v>9.108900951825194E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1215969803646411</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>44043</v>
+        <v>44074</v>
       </c>
       <c r="B8">
-        <v>0.17184506657450169</v>
+        <v>0.0265139299199213</v>
       </c>
       <c r="C8">
-        <v>-4.3350031963752637E-2</v>
+        <v>-0.124521022772221</v>
       </c>
       <c r="D8">
-        <v>3.846144785646044E-2</v>
+        <v>-0.09259263402720985</v>
       </c>
       <c r="E8">
-        <v>4.3292691049889642E-2</v>
+        <v>-0.1011103850390935</v>
       </c>
       <c r="F8">
-        <v>0.1215969803646411</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.07750801818530118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>44074</v>
+        <v>44104</v>
       </c>
       <c r="B9">
-        <v>2.6514007351167601E-2</v>
+        <v>0.03380105244720899</v>
       </c>
       <c r="C9">
-        <v>-0.1245211379963502</v>
+        <v>-0.05579388794871798</v>
       </c>
       <c r="D9">
-        <v>-9.2592477068001E-2</v>
+        <v>-0.0612244583446091</v>
       </c>
       <c r="E9">
-        <v>-0.1011104551985111</v>
+        <v>-0.09882960657041284</v>
       </c>
       <c r="F9">
-        <v>-7.7508018185301175E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.03280124938211948</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>44104</v>
+        <v>44135</v>
       </c>
       <c r="B10">
-        <v>3.3800899035030467E-2</v>
+        <v>0.1539591597528704</v>
       </c>
       <c r="C10">
-        <v>-5.5793927820765747E-2</v>
+        <v>-0.0869546783099866</v>
       </c>
       <c r="D10">
-        <v>-6.1224447279584759E-2</v>
+        <v>-0.0782609142934565</v>
       </c>
       <c r="E10">
-        <v>-9.8829692335394514E-2</v>
+        <v>0.001442938078295652</v>
       </c>
       <c r="F10">
-        <v>3.2801249382119479E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.002038096334578521</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>44135</v>
+        <v>44165</v>
       </c>
       <c r="B11">
-        <v>0.1539594628464149</v>
+        <v>0.2718185639580233</v>
       </c>
       <c r="C11">
-        <v>-8.6954667434717914E-2</v>
+        <v>0.1002142112623747</v>
       </c>
       <c r="D11">
-        <v>-7.826105578232978E-2</v>
+        <v>0.2316038551862794</v>
       </c>
       <c r="E11">
-        <v>1.4431981610765201E-3</v>
+        <v>0.2725520596802764</v>
       </c>
       <c r="F11">
-        <v>2.0380963345785208E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.02542368321522348</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>44165</v>
+        <v>44196</v>
       </c>
       <c r="B12">
-        <v>0.27181857562677952</v>
+        <v>0.04291491462268859</v>
       </c>
       <c r="C12">
-        <v>0.100214201998976</v>
+        <v>0.08398445779794184</v>
       </c>
       <c r="D12">
-        <v>0.23160395080382751</v>
+        <v>0.00727689550489119</v>
       </c>
       <c r="E12">
-        <v>0.27255186313604929</v>
+        <v>0.103428088582374</v>
       </c>
       <c r="F12">
-        <v>2.5423765993740851E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1917354493920431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>44196</v>
+        <v>44227</v>
       </c>
       <c r="B13">
-        <v>4.29146077906426E-2</v>
+        <v>0.03768583997518848</v>
       </c>
       <c r="C13">
-        <v>8.39847162003442E-2</v>
+        <v>-0.02615816811954164</v>
       </c>
       <c r="D13">
-        <v>7.2768900145723237E-3</v>
+        <v>-0.04353602763776576</v>
       </c>
       <c r="E13">
-        <v>0.1034282994998892</v>
+        <v>0.06319130503016246</v>
       </c>
       <c r="F13">
-        <v>0.19173535318782339</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.07073520195368155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>44227</v>
+        <v>44255</v>
       </c>
       <c r="B14">
-        <v>3.7686034250323568E-2</v>
+        <v>0.05221824643384942</v>
       </c>
       <c r="C14">
-        <v>-2.6158386769209781E-2</v>
+        <v>-0.0695068046773375</v>
       </c>
       <c r="D14">
-        <v>-4.3536203932106332E-2</v>
+        <v>0.192208203906685</v>
       </c>
       <c r="E14">
-        <v>6.3191174061240085E-2</v>
+        <v>0.1188706490621048</v>
       </c>
       <c r="F14">
-        <v>7.0735269692004721E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.05712417094928091</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>44255</v>
+        <v>44286</v>
       </c>
       <c r="B15">
-        <v>5.2218149757587762E-2</v>
+        <v>-0.009887991687241193</v>
       </c>
       <c r="C15">
-        <v>-6.9506755345079774E-2</v>
+        <v>0.07416880278457283</v>
       </c>
       <c r="D15">
-        <v>0.1922084715457579</v>
+        <v>0.09103029027247533</v>
       </c>
       <c r="E15">
-        <v>0.1188706490621048</v>
+        <v>0.09915897832269116</v>
       </c>
       <c r="F15">
-        <v>5.7124104072041833E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.09030770516051212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>44286</v>
+        <v>44316</v>
       </c>
       <c r="B16">
-        <v>-9.8878170494508533E-3</v>
+        <v>-0.005906234525248411</v>
       </c>
       <c r="C16">
-        <v>7.4168645536311972E-2</v>
+        <v>-0.09372338293061189</v>
       </c>
       <c r="D16">
-        <v>9.1030407518442491E-2</v>
+        <v>-0.01894857776233705</v>
       </c>
       <c r="E16">
-        <v>9.915897832269116E-2</v>
+        <v>-0.07094672542088398</v>
       </c>
       <c r="F16">
-        <v>9.0307705160512119E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.1398066647624195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>44316</v>
+        <v>44347</v>
       </c>
       <c r="B17">
-        <v>-5.9063216744067448E-3</v>
+        <v>-0.1776639131928278</v>
       </c>
       <c r="C17">
-        <v>-9.3723285906159082E-2</v>
+        <v>-0.2941723148966983</v>
       </c>
       <c r="D17">
-        <v>-1.8948761190730749E-2</v>
+        <v>0.01983924253928815</v>
       </c>
       <c r="E17">
-        <v>-7.0946725420883983E-2</v>
+        <v>-0.0382193843812767</v>
       </c>
       <c r="F17">
-        <v>-0.13980666476241951</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.04493805018020591</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>44347</v>
+        <v>44377</v>
       </c>
       <c r="B18">
-        <v>-0.1776639861462829</v>
+        <v>0.09697192652187159</v>
       </c>
       <c r="C18">
-        <v>-0.30076577207742949</v>
+        <v>0.09190837516582273</v>
       </c>
       <c r="D18">
-        <v>2.056660442649871E-2</v>
+        <v>-0.0010694703618922</v>
       </c>
       <c r="E18">
-        <v>-3.8219485787466263E-2</v>
+        <v>-0.07106114996599167</v>
       </c>
       <c r="F18">
-        <v>-4.4938050180205913E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.01094388475538766</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>44377</v>
+        <v>44408</v>
       </c>
       <c r="B19">
-        <v>9.6972034403428387E-2</v>
+        <v>0.003591849531568547</v>
       </c>
       <c r="C19">
-        <v>9.1908375165822731E-2</v>
+        <v>0.02185433922982472</v>
       </c>
       <c r="D19">
-        <v>-1.0695772046221961E-3</v>
+        <v>-0.09755577337161248</v>
       </c>
       <c r="E19">
-        <v>-7.1061157458387592E-2</v>
+        <v>-0.01660809614751191</v>
       </c>
       <c r="F19">
-        <v>-1.094388475538766E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.09405262212898446</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>44408</v>
+        <v>44439</v>
       </c>
       <c r="B20">
-        <v>3.5915541437605558E-3</v>
+        <v>0.09789479914495325</v>
       </c>
       <c r="C20">
-        <v>2.1854276293637561E-2</v>
+        <v>0.1220350182023602</v>
       </c>
       <c r="D20">
-        <v>-9.7555680295541181E-2</v>
+        <v>0.03898308019428898</v>
       </c>
       <c r="E20">
-        <v>-1.660798453111589E-2</v>
+        <v>0.07727740223867641</v>
       </c>
       <c r="F20">
-        <v>-9.4052622128984464E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.09908403326005244</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>44439</v>
+        <v>44469</v>
       </c>
       <c r="B21">
-        <v>9.7894916323854719E-2</v>
+        <v>0.0363093091187372</v>
       </c>
       <c r="C21">
-        <v>0.1220350873086971</v>
+        <v>-0.05851103538525049</v>
       </c>
       <c r="D21">
-        <v>3.89829893321465E-2</v>
+        <v>-0.06337420330321208</v>
       </c>
       <c r="E21">
-        <v>7.7277402238676407E-2</v>
+        <v>-0.06080764080273171</v>
       </c>
       <c r="F21">
-        <v>9.9083958696643437E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.0651479010546625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>44469</v>
+        <v>44500</v>
       </c>
       <c r="B22">
-        <v>3.6309490870078287E-2</v>
+        <v>0.02177962183600113</v>
       </c>
       <c r="C22">
-        <v>-5.8510925602269448E-2</v>
+        <v>-0.04907963119948788</v>
       </c>
       <c r="D22">
-        <v>-6.3374122856957316E-2</v>
+        <v>-0.2078873139690591</v>
       </c>
       <c r="E22">
-        <v>-6.0807640802731711E-2</v>
+        <v>-0.103692511624299</v>
       </c>
       <c r="F22">
-        <v>-6.5147837632975159E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.04900172808881997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>44500</v>
+        <v>44530</v>
       </c>
       <c r="B23">
-        <v>2.177953383215803E-2</v>
+        <v>0.1342683975444343</v>
       </c>
       <c r="C23">
-        <v>-4.9079742082211442E-2</v>
+        <v>0.1913841894075512</v>
       </c>
       <c r="D23">
-        <v>-0.20788731108647021</v>
+        <v>0.1379801177725761</v>
       </c>
       <c r="E23">
-        <v>-0.10369245458652181</v>
+        <v>-0.0005642639133659477</v>
       </c>
       <c r="F23">
-        <v>-4.9001728088819967E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.04635924717512108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>44530</v>
+        <v>44561</v>
       </c>
       <c r="B24">
-        <v>0.1342684818365982</v>
+        <v>-0.1675097604172054</v>
       </c>
       <c r="C24">
-        <v>0.1913843120315952</v>
+        <v>-0.1242936852925463</v>
       </c>
       <c r="D24">
-        <v>0.13798010161407431</v>
+        <v>0.08554683101652394</v>
       </c>
       <c r="E24">
-        <v>-5.6432751384905E-4</v>
+        <v>-0.08018058234833847</v>
       </c>
       <c r="F24">
-        <v>-4.6359247175121077E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.07914151302420169</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>44561</v>
+        <v>44592</v>
       </c>
       <c r="B25">
-        <v>-0.1675098965971045</v>
+        <v>0.07376564576161271</v>
       </c>
       <c r="C25">
-        <v>-0.1242937754252169</v>
+        <v>0.2387096076569488</v>
       </c>
       <c r="D25">
-        <v>8.5546851680331271E-2</v>
+        <v>0.02554871822432414</v>
       </c>
       <c r="E25">
-        <v>-8.0180582348338469E-2</v>
+        <v>0.2326578265671209</v>
       </c>
       <c r="F25">
-        <v>7.9141433006251871E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.02034621502815859</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>44592</v>
+        <v>44620</v>
       </c>
       <c r="B26">
-        <v>7.3765652346470478E-2</v>
+        <v>0.2221606378299297</v>
       </c>
       <c r="C26">
-        <v>0.23870960765694879</v>
+        <v>-0.1223958442055292</v>
       </c>
       <c r="D26">
-        <v>2.5548706134613349E-2</v>
+        <v>-0.07719291901929448</v>
       </c>
       <c r="E26">
-        <v>0.23265796501238881</v>
+        <v>-0.02788834821967578</v>
       </c>
       <c r="F26">
-        <v>2.0346290686463989E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.07738101077733539</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>44620</v>
+        <v>44651</v>
       </c>
       <c r="B27">
-        <v>0.22216057316442561</v>
+        <v>0.2934418686784723</v>
       </c>
       <c r="C27">
-        <v>-0.12239584420552919</v>
+        <v>0.03743048566941987</v>
       </c>
       <c r="D27">
-        <v>-7.7192945197994356E-2</v>
+        <v>-0.04376432003585973</v>
       </c>
       <c r="E27">
-        <v>-2.7888457401834991E-2</v>
+        <v>0.157274603481417</v>
       </c>
       <c r="F27">
-        <v>-7.7381010777335391E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.04838708788125223</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>44651</v>
+        <v>44681</v>
       </c>
       <c r="B28">
-        <v>0.29344231673672327</v>
+        <v>-0.1367106477722233</v>
       </c>
       <c r="C28">
-        <v>3.7430485669419873E-2</v>
+        <v>-0.1070897400236551</v>
       </c>
       <c r="D28">
-        <v>-4.3764355353129392E-2</v>
+        <v>-0.04099812148979454</v>
       </c>
       <c r="E28">
-        <v>0.157274603481417</v>
+        <v>-0.08855118687392816</v>
       </c>
       <c r="F28">
-        <v>4.8387087881252233E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.03538452904210843</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>44681</v>
+        <v>44712</v>
       </c>
       <c r="B29">
-        <v>-0.13671072419451849</v>
+        <v>0.4386178213474232</v>
       </c>
       <c r="C29">
-        <v>-0.10708974002365509</v>
+        <v>0.1516000535492921</v>
       </c>
       <c r="D29">
-        <v>-2.839834740578806E-2</v>
+        <v>0.007098148148530381</v>
       </c>
       <c r="E29">
-        <v>-8.8551186873928156E-2</v>
+        <v>0.02314802441479036</v>
       </c>
       <c r="F29">
-        <v>-3.5384529042108433E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.04309166187274149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>44712</v>
+        <v>44742</v>
       </c>
       <c r="B30">
-        <v>0.43861764606978948</v>
+        <v>-0.1908576736500071</v>
       </c>
       <c r="C30">
-        <v>0.15159993683331099</v>
+        <v>-0.1452472344567127</v>
       </c>
       <c r="D30">
-        <v>7.098148148530381E-3</v>
+        <v>-0.1086235803635663</v>
       </c>
       <c r="E30">
-        <v>2.3148024414790361E-2</v>
+        <v>-0.1809953859802702</v>
       </c>
       <c r="F30">
-        <v>4.3091661872741487E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.03516823350987841</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>44742</v>
+        <v>44773</v>
       </c>
       <c r="B31">
-        <v>-0.19085775834069929</v>
+        <v>0.1776607039834677</v>
       </c>
       <c r="C31">
-        <v>-0.14524714782653469</v>
+        <v>0.2309516791093886</v>
       </c>
       <c r="D31">
-        <v>-0.1086235803635663</v>
+        <v>-0.06511622693181252</v>
       </c>
       <c r="E31">
-        <v>-0.18099538598027021</v>
+        <v>-0.03990184338417324</v>
       </c>
       <c r="F31">
-        <v>3.516823350987841E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.09010341247088105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>44773</v>
+        <v>44804</v>
       </c>
       <c r="B32">
-        <v>0.1776608272459734</v>
+        <v>0.01331709960846017</v>
       </c>
       <c r="C32">
-        <v>0.2309516791093886</v>
+        <v>0.08027499759905443</v>
       </c>
       <c r="D32">
-        <v>-6.5116226931812515E-2</v>
+        <v>0.05074627526453201</v>
       </c>
       <c r="E32">
-        <v>-3.9901843384173241E-2</v>
+        <v>0.02557554733072243</v>
       </c>
       <c r="F32">
-        <v>9.010341247088105E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.0475609817425986</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>44804</v>
+        <v>44834</v>
       </c>
       <c r="B33">
-        <v>1.3316921853972151E-2</v>
+        <v>-0.0715793122387417</v>
       </c>
       <c r="C33">
-        <v>8.0275093925853636E-2</v>
+        <v>-0.04278282195634864</v>
       </c>
       <c r="D33">
-        <v>5.0746275264532008E-2</v>
+        <v>-0.08617423244928735</v>
       </c>
       <c r="E33">
-        <v>2.5575547330722429E-2</v>
+        <v>-0.1265586384588022</v>
       </c>
       <c r="F33">
-        <v>4.7560981742598603E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.1978786486840899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>44834</v>
+        <v>44865</v>
       </c>
       <c r="B34">
-        <v>-7.1579149376619799E-2</v>
+        <v>0.03228654917005458</v>
       </c>
       <c r="C34">
-        <v>-4.2782996478992863E-2</v>
+        <v>0.05884847281183636</v>
       </c>
       <c r="D34">
-        <v>-8.6174232449287347E-2</v>
+        <v>-0.03221651819948979</v>
       </c>
       <c r="E34">
-        <v>-0.12655863845880219</v>
+        <v>0.02997853855631449</v>
       </c>
       <c r="F34">
-        <v>-0.19787864868408989</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.04850667902074268</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>44865</v>
+        <v>44895</v>
       </c>
       <c r="B35">
-        <v>3.2286643641464829E-2</v>
+        <v>0.0584970787426673</v>
       </c>
       <c r="C35">
-        <v>5.8848571448000708E-2</v>
+        <v>0.03517596781594956</v>
       </c>
       <c r="D35">
-        <v>-3.2216518199489792E-2</v>
+        <v>-0.1381179759779289</v>
       </c>
       <c r="E35">
-        <v>2.997853855631449E-2</v>
+        <v>0.08177404204528838</v>
       </c>
       <c r="F35">
-        <v>4.8506679020742682E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.04275595864152859</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>44895</v>
+        <v>44926</v>
       </c>
       <c r="B36">
-        <v>5.8496890355921087E-2</v>
+        <v>-0.1679802534443341</v>
       </c>
       <c r="C36">
-        <v>3.5175879839079771E-2</v>
+        <v>-0.02215288953615258</v>
       </c>
       <c r="D36">
-        <v>-0.13811797597792891</v>
+        <v>0.03773584905660377</v>
       </c>
       <c r="E36">
-        <v>8.1774042045288375E-2</v>
+        <v>0.01473411908754141</v>
       </c>
       <c r="F36">
-        <v>-4.2755958641528591E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.01690862059076848</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>44926</v>
+        <v>44957</v>
       </c>
       <c r="B37">
-        <v>-0.16798009504963099</v>
+        <v>0.2216933081347203</v>
       </c>
       <c r="C37">
-        <v>-2.215280643150375E-2</v>
+        <v>-0.02613578635809177</v>
       </c>
       <c r="D37">
-        <v>3.7735849056603772E-2</v>
+        <v>0.1212121212121211</v>
       </c>
       <c r="E37">
-        <v>1.473411908754141E-2</v>
+        <v>0.06755053509327325</v>
       </c>
       <c r="F37">
-        <v>1.6908620590768478E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.05119290502721308</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>44957</v>
+        <v>44985</v>
       </c>
       <c r="B38">
-        <v>0.2216931811828855</v>
+        <v>-0.09011679980212128</v>
       </c>
       <c r="C38">
-        <v>-2.6135786358091769E-2</v>
+        <v>0.03784461372080994</v>
       </c>
       <c r="D38">
-        <v>0.1212121212121211</v>
+        <v>-0.01508109427787163</v>
       </c>
       <c r="E38">
-        <v>6.7550535093273245E-2</v>
+        <v>-0.007687696022019352</v>
       </c>
       <c r="F38">
-        <v>-5.1192905027213083E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.004163259424642907</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>44985</v>
+        <v>45016</v>
       </c>
       <c r="B39">
-        <v>-9.0116799802121283E-2</v>
+        <v>-0.08664791662732618</v>
       </c>
       <c r="C39">
-        <v>3.7844613720809939E-2</v>
+        <v>0.1378787964778805</v>
       </c>
       <c r="D39">
-        <v>-1.508109427787163E-2</v>
+        <v>0.003238035504701253</v>
       </c>
       <c r="E39">
-        <v>-7.6876960220193524E-3</v>
+        <v>0.06257439399822839</v>
       </c>
       <c r="F39">
-        <v>-4.1632594246429067E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.06187288907957034</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45016</v>
+        <v>45046</v>
       </c>
       <c r="B40">
-        <v>-8.664782314511188E-2</v>
+        <v>-0.1675302164819408</v>
       </c>
       <c r="C40">
-        <v>0.13787879647788051</v>
+        <v>0.1197827779916865</v>
       </c>
       <c r="D40">
-        <v>3.2380355047012528E-3</v>
+        <v>-0.05306345733041573</v>
       </c>
       <c r="E40">
-        <v>6.2574393998228395E-2</v>
+        <v>0.1499902519243119</v>
       </c>
       <c r="F40">
-        <v>-6.1872889079570337E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.001247776568348957</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45046</v>
+        <v>45077</v>
       </c>
       <c r="B41">
-        <v>-0.16753019933510949</v>
+        <v>-0.004042169030582077</v>
       </c>
       <c r="C41">
-        <v>0.1197827779916865</v>
+        <v>0.08196725294339635</v>
       </c>
       <c r="D41">
-        <v>-5.3063457330415731E-2</v>
+        <v>0.03119584055459268</v>
       </c>
       <c r="E41">
-        <v>0.1499902519243119</v>
+        <v>-0.09295029598469606</v>
       </c>
       <c r="F41">
-        <v>1.247776568348957E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.04153460427357936</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45077</v>
+        <v>45107</v>
       </c>
       <c r="B42">
-        <v>-4.0422914818216693E-3</v>
+        <v>0.1316814654173395</v>
       </c>
       <c r="C42">
-        <v>8.1967252943396351E-2</v>
+        <v>0.05303037674589994</v>
       </c>
       <c r="D42">
-        <v>3.119584055459268E-2</v>
+        <v>0.07843137254901955</v>
       </c>
       <c r="E42">
-        <v>-9.2950295984696063E-2</v>
+        <v>0.08520425553010424</v>
       </c>
       <c r="F42">
-        <v>4.1534604273579363E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.01709398071020707</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45107</v>
+        <v>45138</v>
       </c>
       <c r="B43">
-        <v>0.13168158886456641</v>
+        <v>0.02480733212396635</v>
       </c>
       <c r="C43">
-        <v>5.3030376745899943E-2</v>
+        <v>0.05755393126608999</v>
       </c>
       <c r="D43">
-        <v>7.8431372549019551E-2</v>
+        <v>0.2051948051948052</v>
       </c>
       <c r="E43">
-        <v>8.5204255530104245E-2</v>
+        <v>0.1193634330045448</v>
       </c>
       <c r="F43">
-        <v>1.7093980710207068E-2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.08151261911045804</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45138</v>
+        <v>45169</v>
       </c>
       <c r="B44">
-        <v>2.480711125190083E-2</v>
+        <v>-0.1506310920347296</v>
       </c>
       <c r="C44">
-        <v>5.7553931266089993E-2</v>
+        <v>-0.01023817341200273</v>
       </c>
       <c r="D44">
-        <v>0.20519480519480521</v>
+        <v>-0.09478444066540948</v>
       </c>
       <c r="E44">
-        <v>0.1193634330045448</v>
+        <v>-0.09336497415956257</v>
       </c>
       <c r="F44">
-        <v>8.151261911045804E-2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.04304581690327025</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45169</v>
+        <v>45199</v>
       </c>
       <c r="B45">
-        <v>-0.15063105484703901</v>
+        <v>-0.04665286732202067</v>
       </c>
       <c r="C45">
-        <v>-1.023817341200273E-2</v>
+        <v>-0.07910917520250782</v>
       </c>
       <c r="D45">
-        <v>-9.4784440665409475E-2</v>
+        <v>-0.05442600043478207</v>
       </c>
       <c r="E45">
-        <v>-9.3364974159562575E-2</v>
+        <v>-0.04129634446321917</v>
       </c>
       <c r="F45">
-        <v>-4.3045816903270251E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.02305939362490927</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45199</v>
+        <v>45230</v>
       </c>
       <c r="B46">
-        <v>-4.6652807585537907E-2</v>
+        <v>-0.1888720681337202</v>
       </c>
       <c r="C46">
-        <v>-7.910917520250782E-2</v>
+        <v>-0.02601039916987546</v>
       </c>
       <c r="D46">
-        <v>-5.4426000434782067E-2</v>
+        <v>-0.08223388297552559</v>
       </c>
       <c r="E46">
-        <v>-4.129634446321917E-2</v>
+        <v>-0.05125414724634336</v>
       </c>
       <c r="F46">
-        <v>2.3059393624909271E-2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.05952382059619388</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45230</v>
+        <v>45260</v>
       </c>
       <c r="B47">
-        <v>-0.1888721338597639</v>
+        <v>0.05150642453802323</v>
       </c>
       <c r="C47">
-        <v>-2.6010399169875461E-2</v>
+        <v>0.02302688797295183</v>
       </c>
       <c r="D47">
-        <v>-8.2233882975525585E-2</v>
+        <v>0.1171467764060357</v>
       </c>
       <c r="E47">
-        <v>-5.1254147246343362E-2</v>
+        <v>0.1247127092983267</v>
       </c>
       <c r="F47">
-        <v>-5.9523820596193877E-2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.08941770769043256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45260</v>
+        <v>45291</v>
       </c>
       <c r="B48">
-        <v>5.150650974204618E-2</v>
+        <v>0.2110811650987008</v>
       </c>
       <c r="C48">
-        <v>2.302688797295183E-2</v>
+        <v>0.09147881297500993</v>
       </c>
       <c r="D48">
-        <v>0.1171467764060357</v>
+        <v>0.08055009823182702</v>
       </c>
       <c r="E48">
-        <v>0.1247127092983267</v>
+        <v>-0.004087972086186831</v>
       </c>
       <c r="F48">
-        <v>8.9417707690432557E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.006940544899496026</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45291</v>
+        <v>45322</v>
       </c>
       <c r="B49">
-        <v>0.21108116509870081</v>
+        <v>-0.3013949001706561</v>
       </c>
       <c r="C49">
-        <v>9.1478812975009927E-2</v>
+        <v>-0.009135594566828775</v>
       </c>
       <c r="D49">
-        <v>8.0550098231827016E-2</v>
+        <v>0.004499955610795414</v>
       </c>
       <c r="E49">
-        <v>-4.0879720861868307E-3</v>
+        <v>-0.0620829995016503</v>
       </c>
       <c r="F49">
-        <v>-6.9405448994960262E-3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.07783148314283717</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>45322</v>
+        <v>45351</v>
       </c>
       <c r="B50">
-        <v>-0.30139490017065612</v>
+        <v>0.181839817865715</v>
       </c>
       <c r="C50">
-        <v>-9.1355945668287752E-3</v>
+        <v>0.007092154094970216</v>
       </c>
       <c r="D50">
-        <v>4.4999556107954142E-3</v>
+        <v>0.1086474991023836</v>
       </c>
       <c r="E50">
-        <v>-6.2082999501650298E-2</v>
+        <v>0.07385111238541975</v>
       </c>
       <c r="F50">
-        <v>-7.7831483142837166E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.04887415088293801</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>45351</v>
+        <v>45382</v>
       </c>
       <c r="B51">
-        <v>0.18183981786571499</v>
+        <v>-0.0112631409154984</v>
       </c>
       <c r="C51">
-        <v>7.0921540949702164E-3</v>
+        <v>0.007042209658900234</v>
       </c>
       <c r="D51">
-        <v>0.1086474991023836</v>
+        <v>0.050204081632653</v>
       </c>
       <c r="E51">
-        <v>7.3851112385419748E-2</v>
+        <v>0.01018849031268765</v>
       </c>
       <c r="F51">
-        <v>4.8874150882938013E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1353226039800377</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>45382</v>
+        <v>45412</v>
       </c>
       <c r="B52">
-        <v>-1.1263140915498401E-2</v>
+        <v>-0.07058586207845341</v>
       </c>
       <c r="C52">
-        <v>7.0422096589002336E-3</v>
+        <v>-0.04195800735730948</v>
       </c>
       <c r="D52">
-        <v>5.0204081632652997E-2</v>
+        <v>-0.001165954139137226</v>
       </c>
       <c r="E52">
-        <v>1.018849031268765E-2</v>
+        <v>-0.05461827799224861</v>
       </c>
       <c r="F52">
-        <v>0.1353226039800377</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.02670837902762091</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>45412</v>
+        <v>45443</v>
       </c>
       <c r="B53">
-        <v>-7.058586207845341E-2</v>
+        <v>0.02669014896583533</v>
       </c>
       <c r="C53">
-        <v>-4.1958007357309479E-2</v>
+        <v>0.04617165138707691</v>
       </c>
       <c r="D53">
-        <v>-1.1659541391372259E-3</v>
+        <v>0.08210116731517503</v>
       </c>
       <c r="E53">
-        <v>-5.4618277992248609E-2</v>
+        <v>0.05005559741067334</v>
       </c>
       <c r="F53">
-        <v>-2.670837902762091E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.1121734132019911</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>45443</v>
+        <v>45473</v>
       </c>
       <c r="B54">
-        <v>2.6690148965835329E-2</v>
+        <v>-0.1274090078315652</v>
       </c>
       <c r="C54">
-        <v>4.6171651387076913E-2</v>
+        <v>-0.05514705882352944</v>
       </c>
       <c r="D54">
-        <v>8.2101167315175028E-2</v>
+        <v>0.0431499460625675</v>
       </c>
       <c r="E54">
-        <v>5.0055597410673343E-2</v>
+        <v>-0.002648264792534882</v>
       </c>
       <c r="F54">
-        <v>0.1121734132019911</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.04849398771678837</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>45473</v>
+        <v>45504</v>
       </c>
       <c r="B55">
-        <v>-0.1274090078315652</v>
+        <v>-0.06601223623825725</v>
       </c>
       <c r="C55">
-        <v>-5.5147058823529438E-2</v>
+        <v>0.08910503461667063</v>
       </c>
       <c r="D55">
-        <v>4.3149946062567501E-2</v>
+        <v>0.07549120992761127</v>
       </c>
       <c r="E55">
-        <v>-2.6482647925348819E-3</v>
+        <v>0.06638343096466559</v>
       </c>
       <c r="F55">
-        <v>-4.8493987716788367E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.09517238025712993</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>45504</v>
+        <v>45535</v>
       </c>
       <c r="B56">
-        <v>-6.6012236238257249E-2</v>
+        <v>0.0194429279313908</v>
       </c>
       <c r="C56">
-        <v>8.9105034616670631E-2</v>
+        <v>-0.01036082157814155</v>
       </c>
       <c r="D56">
-        <v>7.5491209927611269E-2</v>
+        <v>0.03525641025641035</v>
       </c>
       <c r="E56">
-        <v>6.6383430964665591E-2</v>
+        <v>0.02838643909312411</v>
       </c>
       <c r="F56">
-        <v>-9.5172380257129929E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+        <v>-0.08730186672736573</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>45535</v>
+        <v>45565</v>
       </c>
       <c r="B57">
-        <v>1.94429279313908E-2</v>
+        <v>0.07422683311200551</v>
       </c>
       <c r="C57">
-        <v>-1.0360821578141549E-2</v>
+        <v>0.003610108303249149</v>
       </c>
       <c r="D57">
-        <v>3.5256410256410353E-2</v>
+        <v>0.03095975232198134</v>
       </c>
       <c r="E57">
-        <v>2.8386439093124109E-2</v>
+        <v>0.00532690616869802</v>
       </c>
       <c r="F57">
-        <v>-8.7301866727365729E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.005461551591836589</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="B58">
-        <v>7.4226833112005508E-2</v>
+        <v>-0.07893476227059415</v>
       </c>
       <c r="C58">
-        <v>3.6101083032491492E-3</v>
+        <v>-0.01208627824303055</v>
       </c>
       <c r="D58">
-        <v>3.0959752321981341E-2</v>
+        <v>0.03633633633633626</v>
       </c>
       <c r="E58">
-        <v>5.3269061686980201E-3</v>
+        <v>-0.05876682562157198</v>
       </c>
       <c r="F58">
-        <v>5.4615515918365887E-3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+        <v>0.008305670880552229</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>45596</v>
+        <v>45626</v>
       </c>
       <c r="B59">
-        <v>-7.893476227059415E-2</v>
+        <v>0.001823383587838512</v>
       </c>
       <c r="C59">
-        <v>-1.2086278243030549E-2</v>
+        <v>0.07231278871356372</v>
       </c>
       <c r="D59">
-        <v>3.6336336336336261E-2</v>
+        <v>-0.04375543320776587</v>
       </c>
       <c r="E59">
-        <v>-5.8766825621571983E-2</v>
+        <v>-0.02917101205046024</v>
       </c>
       <c r="F59">
-        <v>8.3056708805522295E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="2">
-        <v>45626</v>
-      </c>
-      <c r="B60">
-        <v>1.8233835878385121E-3</v>
-      </c>
-      <c r="C60">
-        <v>7.2312788713563725E-2</v>
-      </c>
-      <c r="D60">
-        <v>-4.375543320776587E-2</v>
-      </c>
-      <c r="E60">
-        <v>-2.917101205046024E-2</v>
-      </c>
-      <c r="F60">
-        <v>-3.130137575302117E-3</v>
+        <v>-0.003130137575302117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>